<commit_message>
WPC: Student class added and Excel updated.
</commit_message>
<xml_diff>
--- a/xmlChecker/data/project_U1_sub1/students_U1.xlsx
+++ b/xmlChecker/data/project_U1_sub1/students_U1.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="MainInfo" sheetId="3" r:id="rId1"/>
@@ -13,12 +13,12 @@
     <sheet name="Results_U1E2_1_sub1" sheetId="2" r:id="rId4"/>
     <sheet name="Results_U1E3_1_sub1" sheetId="6" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="111">
   <si>
     <t>item2</t>
   </si>
@@ -384,6 +384,9 @@
   </si>
   <si>
     <t>U1E2_1</t>
+  </si>
+  <si>
+    <t>StudentSheet</t>
   </si>
 </sst>
 </file>
@@ -602,7 +605,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -637,7 +640,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -846,64 +849,70 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C48"/>
+  <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21.6640625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="45.33203125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="11.7109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="21.7109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="45.28515625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="6" t="str">
+        <f>TEXT(ZipFiles_U1_sub1!$E$9,"0")</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="7">
+      <c r="E4" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="B4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>33</v>
       </c>
       <c r="C5" t="str">
-        <f>TEXT($C$2*10-1,"0")</f>
+        <f>TEXT($E$4*10-1,"0")</f>
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>34</v>
       </c>
       <c r="C6" t="str">
-        <f>TEXT($C$2*10 + 8,"0")</f>
+        <f>TEXT($E$4*10 + 8,"0")</f>
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>22</v>
       </c>
@@ -911,7 +920,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
         <v>105</v>
       </c>
@@ -919,7 +928,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>21</v>
       </c>
@@ -927,7 +936,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>24</v>
       </c>
@@ -935,7 +944,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>26</v>
       </c>
@@ -944,7 +953,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>27</v>
       </c>
@@ -952,7 +961,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>28</v>
       </c>
@@ -960,7 +969,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>29</v>
       </c>
@@ -968,7 +977,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>25</v>
       </c>
@@ -976,7 +985,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="19" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>22</v>
       </c>
@@ -984,7 +993,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
         <v>105</v>
       </c>
@@ -992,7 +1001,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="21" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>21</v>
       </c>
@@ -1000,7 +1009,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="22" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>24</v>
       </c>
@@ -1008,7 +1017,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="23" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>26</v>
       </c>
@@ -1017,7 +1026,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>27</v>
       </c>
@@ -1025,7 +1034,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="25" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>28</v>
       </c>
@@ -1033,7 +1042,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="26" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>29</v>
       </c>
@@ -1041,7 +1050,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>25</v>
       </c>
@@ -1049,7 +1058,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>22</v>
       </c>
@@ -1057,7 +1066,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="30" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B30" s="2" t="s">
         <v>105</v>
       </c>
@@ -1065,7 +1074,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="31" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>21</v>
       </c>
@@ -1073,7 +1082,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="32" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>24</v>
       </c>
@@ -1081,7 +1090,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>26</v>
       </c>
@@ -1090,7 +1099,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>27</v>
       </c>
@@ -1098,7 +1107,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>28</v>
       </c>
@@ -1106,7 +1115,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>29</v>
       </c>
@@ -1114,7 +1123,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>25</v>
       </c>
@@ -1122,7 +1131,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>22</v>
       </c>
@@ -1130,39 +1139,39 @@
         <v>23</v>
       </c>
     </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
     </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B41" s="10"/>
       <c r="C41" s="11"/>
     </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B42" s="12"/>
       <c r="C42" s="13"/>
     </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B43" s="12"/>
       <c r="C43" s="13"/>
     </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B44" s="12"/>
       <c r="C44" s="13"/>
     </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B45" s="12"/>
       <c r="C45" s="13"/>
     </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B46" s="12"/>
       <c r="C46" s="13"/>
     </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B47" s="12"/>
       <c r="C47" s="13"/>
     </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B48" s="14"/>
       <c r="C48" s="15"/>
     </row>
@@ -1180,9 +1189,9 @@
       <selection activeCell="A12" sqref="A12:A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="29.88671875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="29.85546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1268,7 +1277,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>3</v>
       </c>
@@ -1285,7 +1294,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>4</v>
       </c>
@@ -1315,19 +1324,19 @@
       <selection activeCell="AC20" sqref="AC20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="7" max="7" width="18.33203125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="20.6640625" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="12.6640625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="18.28515625" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="20.7109375" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="12.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="9" spans="1:37" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
       <c r="G9" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:37" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
@@ -1466,37 +1475,37 @@
       <selection activeCell="A9" sqref="A9:AH10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="13.33203125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="30.6640625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="32.44140625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="37.109375" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="32.6640625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="29.109375" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="30.5546875" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="8.88671875" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="10.44140625" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="9.33203125" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="10.88671875" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="12.44140625" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="12.88671875" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="30.5546875" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="26.88671875" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="29.109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="13.28515625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="30.7109375" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="32.42578125" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="37.140625" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="32.7109375" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="29.140625" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="30.5703125" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="8.85546875" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="10.42578125" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="9.28515625" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="10.85546875" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="12.42578125" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="12.85546875" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="30.5703125" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="26.85546875" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="29.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:34" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:34" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
       <c r="G9" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:34" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
@@ -1770,7 +1779,7 @@
       <c r="AD14" s="4"/>
       <c r="AE14" s="4"/>
     </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
       <c r="L15" s="4"/>
     </row>
   </sheetData>
@@ -1786,7 +1795,7 @@
       <selection activeCell="AA13" sqref="AA13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="9" spans="1:34" x14ac:dyDescent="0.25">
       <c r="G9" t="s">

</xml_diff>